<commit_message>
feat: implement 13 PRSB alignment profiles and terminology
</commit_message>
<xml_diff>
--- a/temp/pages/StructureDefinition-intervention-goal-reference.xlsx
+++ b/temp/pages/StructureDefinition-intervention-goal-reference.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-26T15:22:58+00:00</t>
+    <t>2026-01-01T13:37:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Extension to link nursing interventions to the patient goals they are intended to achieve. Supports goal-directed care planning and intervention tracking.</t>
+    <t>Extension to link nursing interventions to the patient goals they are intended to achieve.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -319,7 +319,7 @@
     <t>Extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://clinyqai.github.io/open-nursing-core-ig/StructureDefinition/onc-patient-goal)
+    <t xml:space="preserve">Reference(https://clinyqai.github.io/open-nursing-core-ig/StructureDefinition/onc-nursing-goal)
 </t>
   </si>
   <si>
@@ -652,7 +652,7 @@
     <col min="8" max="8" width="13.1171875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="10.75390625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="78.00390625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="78.18359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>